<commit_message>
Finished migrating contingent WMO assumptions to consolidated input spreadsheet
</commit_message>
<xml_diff>
--- a/CaUWMET/tests/CaUWMET_CPED example for Python test.xlsx
+++ b/CaUWMET/tests/CaUWMET_CPED example for Python test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KD012200\GitHub_Repos\California-Urban-Water-Management-Economic-Tool\CaUWMET\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1D6D76-B7F5-4B1D-9F30-D2F8ED80F700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9107EF29-3F66-485E-8399-9653701572A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,7 +89,7 @@
     <definedName name="use_2" localSheetId="0">'CPED Calc_trial'!$I$10</definedName>
     <definedName name="use_3" localSheetId="0">'CPED Calc_trial'!$H$10</definedName>
   </definedNames>
-  <calcPr calcId="191028" iterate="1" iterateCount="1000"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1179,61 +1179,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49058502.392924607</c:v>
+                  <c:v>49358404.165062651</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>107548140.87291643</c:v>
+                  <c:v>109128127.49468267</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>177781681.71136856</c:v>
+                  <c:v>182510508.36343467</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>262772154.91537166</c:v>
+                  <c:v>274091646.10037959</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>366491430.72424567</c:v>
+                  <c:v>390661709.97357905</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>494245158.94430643</c:v>
+                  <c:v>542678230.74601614</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>653228433.90731168</c:v>
+                  <c:v>747027886.28187668</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>853371068.88973713</c:v>
+                  <c:v>1032585067.1571265</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1108665366.9296954</c:v>
+                  <c:v>1452276952.3033276</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1439338897.8280289</c:v>
+                  <c:v>2111735995.912674</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1875608810.4274888</c:v>
+                  <c:v>3245209065.149663</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2464680250.0551219</c:v>
+                  <c:v>5446191401.7889786</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3136169175.4372315</c:v>
+                  <c:v>6811179261.5289164</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3997692702.3955197</c:v>
+                  <c:v>7562346275.6050835</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5205177019.6790686</c:v>
+                  <c:v>8621644976.4583035</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6942461766.0623312</c:v>
+                  <c:v>10159289752.628944</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9520867655.2637615</c:v>
+                  <c:v>12467547337.625431</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13493246564.177263</c:v>
+                  <c:v>16072367376.036104</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>26403482129.485783</c:v>
+                  <c:v>27784752608.754646</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1823,8 +1823,8 @@
   </sheetPr>
   <dimension ref="A1:BA68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="AF16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AZ38" sqref="AZ38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2145,16 +2145,16 @@
         <v>-0.2</v>
       </c>
       <c r="R9" s="102">
-        <v>-0.12</v>
+        <v>-0.2</v>
       </c>
       <c r="S9" s="102">
-        <v>-0.1</v>
+        <v>-0.2</v>
       </c>
       <c r="T9" s="102">
-        <v>-0.11</v>
+        <v>-0.2</v>
       </c>
       <c r="U9" s="103">
-        <v>-0.4</v>
+        <v>-0.2</v>
       </c>
       <c r="V9" s="13"/>
       <c r="W9" s="13"/>
@@ -2204,19 +2204,19 @@
       </c>
       <c r="R10" s="131">
         <f>base_use_mf/(p1_base^elasticity_mf)</f>
-        <v>1223679.7878046185</v>
+        <v>2054474.9728149578</v>
       </c>
       <c r="S10" s="13">
         <f>base_use_ind/(p1_base^elasticity_ind)</f>
-        <v>430001.04479625466</v>
+        <v>821789.98912598309</v>
       </c>
       <c r="T10" s="13">
         <f>base_use_comm/(p1_base^elasticity_comm)</f>
-        <v>229386.91925479213</v>
+        <v>410894.99456299155</v>
       </c>
       <c r="U10" s="34">
         <f>base_use_lndscp/(p1_base^elasticity_lndscp)</f>
-        <v>3001535.7319248011</v>
+        <v>821789.98912598309</v>
       </c>
       <c r="V10" s="132">
         <f>size_sf*base_use_total</f>
@@ -2764,27 +2764,27 @@
       </c>
       <c r="AF20" s="64">
         <f t="shared" ref="AF20:AF37" si="16">IF(shortage_MF&lt;=lowerbound_MF,((elasticity_mf*base_use_mf*EXP((LN(base_use_mf/coeff_mf))/elasticity_mf))/(elasticity_mf + 1))-((elasticity_mf*(base_use_mf*(1-lowerbound_MF)*EXP((LN((base_use_mf*(1-lowerbound_MF)/coeff_mf))/elasticity_mf))/(elasticity_mf + 1)))), IF(shortage_MF&gt;=upperbound_MF,((elasticity_mf*base_use_mf*EXP((LN(base_use_mf/coeff_mf))/elasticity_mf))/(elasticity_mf + 1))-((elasticity_mf*(base_use_mf*(1-upperbound_MF))*EXP((LN((base_use_mf*(1-upperbound_MF))/coeff_mf))/elasticity_mf))/(elasticity_mf + 1)), ((elasticity_mf*base_use_mf*EXP((LN(base_use_mf/coeff_mf))/elasticity_mf))/(elasticity_mf + 1))-((elasticity_mf*(base_use_mf-shortage_af_MF)*EXP((LN((base_use_mf-shortage_af_MF)/coeff_mf))/elasticity_mf))/(elasticity_mf + 1))))</f>
-        <v>8568471.8775434792</v>
+        <v>8259052.3837222308</v>
       </c>
       <c r="AL20" s="64">
         <f t="shared" ref="AL20:AL37" si="17">IF(shortage_IND&lt;=lowerbound_IND,((elasticity_ind*base_use_ind*EXP((LN(base_use_ind/coeff_ind))/elasticity_ind))/(elasticity_ind + 1))-((elasticity_ind*(base_use_ind*(1-lowerbound_IND)*EXP((LN((base_use_ind*(1-lowerbound_IND)/coeff_ind))/elasticity_ind))/(elasticity_ind + 1)))), IF(shortage_IND&gt;=upperbound_IND,((elasticity_ind*base_use_ind*EXP((LN(base_use_ind/coeff_ind))/elasticity_ind))/(elasticity_ind + 1))-((elasticity_ind*(base_use_ind*(1-upperbound_IND))*EXP((LN((base_use_ind*(1-upperbound_IND))/coeff_ind))/elasticity_ind))/(elasticity_ind + 1)), ((elasticity_ind*base_use_ind*EXP((LN(base_use_ind/coeff_ind))/elasticity_ind))/(elasticity_ind + 1))-((elasticity_ind*(base_use_ind-shortage_af_IND)*EXP((LN((base_use_ind-shortage_af_IND)/coeff_ind))/elasticity_ind))/(elasticity_ind + 1))))</f>
-        <v>1363739.5678167623</v>
+        <v>1333261.4615133703</v>
       </c>
       <c r="AR20" s="64">
         <f t="shared" ref="AR20:AR37" si="18">IF(shortage_COM&lt;=lowerbound_COM,((elasticity_comm*base_use_comm*EXP((LN(base_use_comm/coeff_comm))/elasticity_comm))/(elasticity_comm + 1))-((elasticity_comm*(base_use_comm*(1-lowerbound_COM)*EXP((LN((base_use_comm*(1-lowerbound_COM)/coeff_comm))/elasticity_comm))/(elasticity_comm + 1)))), IF(shortage_COM&gt;=upperbound_COM,((elasticity_comm*base_use_comm*EXP((LN(base_use_comm/coeff_comm))/elasticity_comm))/(elasticity_comm + 1))-((elasticity_comm*(base_use_comm*(1-upperbound_COM))*EXP((LN((base_use_comm*(1-upperbound_COM))/coeff_comm))/elasticity_comm))/(elasticity_comm + 1)), ((elasticity_comm*base_use_comm*EXP((LN(base_use_comm/coeff_comm))/elasticity_comm))/(elasticity_comm + 1))-((elasticity_comm*(base_use_comm-shortage_af_COM)*EXP((LN((base_use_comm-shortage_af_COM)/coeff_comm))/elasticity_comm))/(elasticity_comm + 1))))</f>
-        <v>1570797.6915409286</v>
+        <v>1507214.2319882512</v>
       </c>
       <c r="AX20" s="64">
         <f t="shared" ref="AX20:AX37" si="19">IF(shortage_LNDSCP&lt;=$U$14,((elasticity_lndscp*base_use_lndscp*EXP((LN(base_use_lndscp/coeff_lndscp))/elasticity_lndscp))/(elasticity_lndscp + 1))-((elasticity_lndscp*(base_use_lndscp*(1-low_bound_lndscp)*EXP((LN((base_use_lndscp*(1-low_bound_lndscp)/coeff_lndscp))/elasticity_lndscp))/(elasticity_lndscp + 1)))), IF(shortage_LNDSCP&gt;=upperbound_LNDSCP,((elasticity_lndscp*base_use_lndscp*EXP((LN(base_use_lndscp/coeff_lndscp))/elasticity_lndscp))/(elasticity_lndscp + 1))-((elasticity_lndscp*(base_use_lndscp*(1-upperbound_LNDSCP))*EXP((LN((base_use_lndscp*(1-upperbound_LNDSCP))/coeff_lndscp))/elasticity_lndscp))/(elasticity_lndscp + 1)), ((elasticity_lndscp*base_use_lndscp*EXP((LN(base_use_lndscp/coeff_lndscp))/elasticity_lndscp))/(elasticity_lndscp + 1))-((elasticity_lndscp*(base_use_lndscp-shortage_af_LNDSCP)*EXP((LN((base_use_lndscp-shortage_af_LNDSCP)/coeff_lndscp))/elasticity_lndscp))/(elasticity_lndscp + 1))))</f>
-        <v>8980887.9600099027</v>
+        <v>9684270.7918252647</v>
       </c>
       <c r="AY20" s="48">
         <f t="shared" ref="AY20:AY38" si="20">AZ20/P45</f>
-        <v>708.98105456093754</v>
+        <v>713.31515903424884</v>
       </c>
       <c r="AZ20" s="14">
         <f t="shared" si="14"/>
-        <v>49058502.392924607</v>
+        <v>49358404.165062651</v>
       </c>
       <c r="BA20" s="65">
         <f t="shared" si="15"/>
@@ -2855,27 +2855,27 @@
       </c>
       <c r="AF21" s="64">
         <f t="shared" si="16"/>
-        <v>18849960.653162234</v>
+        <v>17472358.44198361</v>
       </c>
       <c r="AL21" s="64">
         <f t="shared" si="17"/>
-        <v>2855834.6239179652</v>
+        <v>2727853.535294205</v>
       </c>
       <c r="AR21" s="64">
         <f t="shared" si="18"/>
-        <v>3454991.8274118621</v>
+        <v>3173011.0553799421</v>
       </c>
       <c r="AX21" s="64">
         <f t="shared" si="19"/>
-        <v>19430476.255549997</v>
+        <v>22798026.949150555</v>
       </c>
       <c r="AY21" s="48">
         <f t="shared" si="20"/>
-        <v>777.12924990496322</v>
+        <v>788.5460332009568</v>
       </c>
       <c r="AZ21" s="14">
         <f t="shared" si="14"/>
-        <v>107548140.87291643</v>
+        <v>109128127.49468267</v>
       </c>
       <c r="BA21" s="65">
         <f t="shared" si="15"/>
@@ -2946,27 +2946,27 @@
       </c>
       <c r="AF22" s="64">
         <f t="shared" si="16"/>
-        <v>31237333.955084987</v>
+        <v>27775334.673295721</v>
       </c>
       <c r="AL22" s="64">
         <f t="shared" si="17"/>
-        <v>4489699.5597629938</v>
+        <v>4187193.0657581463</v>
       </c>
       <c r="AR22" s="64">
         <f t="shared" si="18"/>
-        <v>5723523.8166936468</v>
+        <v>5017840.9574663974</v>
       </c>
       <c r="AX22" s="64">
         <f t="shared" si="19"/>
-        <v>31708487.68894954</v>
+        <v>40907502.976036981</v>
       </c>
       <c r="AY22" s="48">
         <f t="shared" si="20"/>
-        <v>856.41861609648095</v>
+        <v>879.19855122892966</v>
       </c>
       <c r="AZ22" s="14">
         <f t="shared" si="14"/>
-        <v>177781681.71136856</v>
+        <v>182510508.36343467</v>
       </c>
       <c r="BA22" s="65">
         <f t="shared" si="15"/>
@@ -3037,27 +3037,27 @@
       </c>
       <c r="AF23" s="64">
         <f t="shared" si="16"/>
-        <v>46225693.334588774</v>
+        <v>39326356.824808732</v>
       </c>
       <c r="AL23" s="64">
         <f>IF(shortage_IND&lt;=lowerbound_IND,((elasticity_ind*base_use_ind*EXP((LN(base_use_ind/coeff_ind))/elasticity_ind))/(elasticity_ind + 1))-((elasticity_ind*(base_use_ind*(1-lowerbound_IND)*EXP((LN((base_use_ind*(1-lowerbound_IND)/coeff_ind))/elasticity_ind))/(elasticity_ind + 1)))), IF(shortage_IND&gt;=upperbound_IND,((elasticity_ind*base_use_ind*EXP((LN(base_use_ind/coeff_ind))/elasticity_ind))/(elasticity_ind + 1))-((elasticity_ind*(base_use_ind*(1-upperbound_IND))*EXP((LN((base_use_ind*(1-upperbound_IND))/coeff_ind))/elasticity_ind))/(elasticity_ind + 1)), ((elasticity_ind*base_use_ind*EXP((LN(base_use_ind/coeff_ind))/elasticity_ind))/(elasticity_ind + 1))-((elasticity_ind*(base_use_ind-shortage_af_IND)*EXP((LN((base_use_ind-shortage_af_IND)/coeff_ind))/elasticity_ind))/(elasticity_ind + 1))))</f>
-        <v>6280292.7244417835</v>
+        <v>5714921.0592027083</v>
       </c>
       <c r="AR23" s="64">
         <f t="shared" si="18"/>
-        <v>8465384.4106408022</v>
+        <v>7065298.4246141613</v>
       </c>
       <c r="AX23" s="64">
         <f t="shared" si="19"/>
-        <v>46296418.573757976</v>
+        <v>66480703.919811666</v>
       </c>
       <c r="AY23" s="48">
         <f t="shared" si="20"/>
-        <v>949.37916168441518</v>
+        <v>990.27576678847572</v>
       </c>
       <c r="AZ23" s="14">
         <f t="shared" si="14"/>
-        <v>262772154.91537166</v>
+        <v>274091646.10037959</v>
       </c>
       <c r="BA23" s="65">
         <f t="shared" si="15"/>
@@ -3128,27 +3128,27 @@
       </c>
       <c r="AF24" s="64">
         <f t="shared" si="16"/>
-        <v>64442295.962985493</v>
+        <v>52311318.345438704</v>
       </c>
       <c r="AL24" s="64">
         <f t="shared" si="17"/>
-        <v>8244310.7907152753</v>
+        <v>7314919.6494385675</v>
       </c>
       <c r="AR24" s="64">
         <f t="shared" si="18"/>
-        <v>11792735.863012906</v>
+        <v>9342686.6750401706</v>
       </c>
       <c r="AX24" s="64">
         <f t="shared" si="19"/>
-        <v>63852005.849980861</v>
+        <v>103532703.04611048</v>
       </c>
       <c r="AY24" s="48">
         <f t="shared" si="20"/>
-        <v>1059.2882716285169</v>
+        <v>1129.148822747567</v>
       </c>
       <c r="AZ24" s="14">
         <f t="shared" si="14"/>
-        <v>366491430.72424567</v>
+        <v>390661709.97357905</v>
       </c>
       <c r="BA24" s="65">
         <f t="shared" si="15"/>
@@ -3222,27 +3222,27 @@
       </c>
       <c r="AF25" s="64">
         <f t="shared" si="16"/>
-        <v>86686255.531868875</v>
+        <v>66949232.775843337</v>
       </c>
       <c r="AL25" s="64">
         <f t="shared" si="17"/>
-        <v>10400409.727604901</v>
+        <v>8991330.5217283443</v>
       </c>
       <c r="AR25" s="64">
         <f t="shared" si="18"/>
-        <v>15847645.195009496</v>
+        <v>11881699.115892529</v>
       </c>
       <c r="AX25" s="64">
         <f t="shared" si="19"/>
-        <v>85295024.524293244</v>
+        <v>158840144.36702204</v>
       </c>
       <c r="AY25" s="48">
         <f t="shared" si="20"/>
-        <v>1190.4509816783918</v>
+        <v>1307.1080633485481</v>
       </c>
       <c r="AZ25" s="14">
         <f t="shared" si="14"/>
-        <v>494245158.94430643</v>
+        <v>542678230.74601614</v>
       </c>
       <c r="BA25" s="65">
         <f t="shared" si="15"/>
@@ -3313,27 +3313,27 @@
       </c>
       <c r="AF26" s="64">
         <f t="shared" si="16"/>
-        <v>113981570.28413814</v>
+        <v>83499152.601778314</v>
       </c>
       <c r="AL26" s="64">
         <f t="shared" si="17"/>
-        <v>12769456.320098592</v>
+        <v>10748574.935651504</v>
       </c>
       <c r="AR26" s="64">
         <f t="shared" si="18"/>
-        <v>20810987.255893812</v>
+        <v>14719244.957267608</v>
       </c>
       <c r="AX26" s="64">
         <f t="shared" si="19"/>
-        <v>111947219.78011999</v>
+        <v>244341713.52011821</v>
       </c>
       <c r="AY26" s="48">
         <f t="shared" si="20"/>
-        <v>1348.6131319922406</v>
+        <v>1542.2654084085616</v>
       </c>
       <c r="AZ26" s="14">
         <f t="shared" si="14"/>
-        <v>653228433.90731168</v>
+        <v>747027886.28187668</v>
       </c>
       <c r="BA26" s="65">
         <f t="shared" si="15"/>
@@ -3404,27 +3404,27 @@
       </c>
       <c r="AF27" s="64">
         <f t="shared" si="16"/>
-        <v>147648447.96805242</v>
+        <v>102268757.44009249</v>
       </c>
       <c r="AL27" s="64">
         <f t="shared" si="17"/>
-        <v>15374814.80523912</v>
+        <v>12591375.502574869</v>
       </c>
       <c r="AR27" s="64">
         <f t="shared" si="18"/>
-        <v>26914288.915903799</v>
+        <v>17898453.677396886</v>
       </c>
       <c r="AX27" s="64">
         <f t="shared" si="19"/>
-        <v>145770001.96998942</v>
+        <v>382162965.30650985</v>
       </c>
       <c r="AY27" s="48">
         <f t="shared" si="20"/>
-        <v>1541.5878258660928</v>
+        <v>1865.3322414264139</v>
       </c>
       <c r="AZ27" s="14">
         <f t="shared" si="14"/>
-        <v>853371068.88973713</v>
+        <v>1032585067.1571265</v>
       </c>
       <c r="BA27" s="65">
         <f t="shared" si="15"/>
@@ -3495,27 +3495,27 @@
       </c>
       <c r="AF28" s="64">
         <f t="shared" si="16"/>
-        <v>189399946.21605444</v>
+        <v>123625071.31478889</v>
       </c>
       <c r="AL28" s="64">
         <f t="shared" si="17"/>
-        <v>18242673.930189677</v>
+        <v>14524779.890244223</v>
       </c>
       <c r="AR28" s="64">
         <f t="shared" si="18"/>
-        <v>34455586.870899804</v>
+        <v>21469902.443158783</v>
       </c>
       <c r="AX28" s="64">
         <f t="shared" si="19"/>
-        <v>189788153.24580124</v>
+        <v>615878191.98838544</v>
       </c>
       <c r="AY28" s="48">
         <f t="shared" si="20"/>
-        <v>1780.2390177287334</v>
+        <v>2331.9931984512909</v>
       </c>
       <c r="AZ28" s="14">
         <f t="shared" si="14"/>
-        <v>1108665366.9296954</v>
+        <v>1452276952.3033276</v>
       </c>
       <c r="BA28" s="65">
         <f t="shared" si="15"/>
@@ -3586,27 +3586,27 @@
       </c>
       <c r="AF29" s="64">
         <f t="shared" si="16"/>
-        <v>241473925.35487264</v>
+        <v>148007911.98276496</v>
       </c>
       <c r="AL29" s="64">
         <f t="shared" si="17"/>
-        <v>21402420.601556301</v>
+        <v>16554186.645856433</v>
       </c>
       <c r="AR29" s="64">
         <f t="shared" si="18"/>
-        <v>43820801.319632061</v>
+        <v>25493122.854143783</v>
       </c>
       <c r="AX29" s="64">
         <f t="shared" si="19"/>
-        <v>248890352.9232299</v>
+        <v>1037929376.8011708</v>
       </c>
       <c r="AY29" s="48">
         <f t="shared" si="20"/>
-        <v>2080.0961298807811</v>
+        <v>3051.8273903778813</v>
       </c>
       <c r="AZ29" s="14">
         <f t="shared" si="14"/>
-        <v>1439338897.8280289</v>
+        <v>2111735995.912674</v>
       </c>
       <c r="BA29" s="65">
         <f t="shared" si="15"/>
@@ -3677,27 +3677,27 @@
       </c>
       <c r="AF30" s="64">
         <f t="shared" si="16"/>
-        <v>306814681.94322813</v>
+        <v>175946868.53700119</v>
       </c>
       <c r="AL30" s="64">
         <f t="shared" si="17"/>
-        <v>24887067.309836023</v>
+        <v>18685373.350080341</v>
       </c>
       <c r="AR30" s="64">
         <f t="shared" si="18"/>
-        <v>55512746.12551827</v>
+        <v>30038459.458726913</v>
       </c>
       <c r="AX30" s="64">
         <f t="shared" si="19"/>
-        <v>331454043.43875968</v>
+        <v>1863598092.1937079</v>
       </c>
       <c r="AY30" s="48">
         <f t="shared" si="20"/>
-        <v>2464.1657825925381</v>
+        <v>4263.5399723241344</v>
       </c>
       <c r="AZ30" s="14">
         <f t="shared" si="14"/>
-        <v>1875608810.4274888</v>
+        <v>3245209065.149663</v>
       </c>
       <c r="BA30" s="65">
         <f t="shared" si="15"/>
@@ -3768,27 +3768,27 @@
       </c>
       <c r="AF31" s="64">
         <f t="shared" si="16"/>
-        <v>389325110.62179905</v>
+        <v>208082866.37636894</v>
       </c>
       <c r="AL31" s="64">
         <f t="shared" si="17"/>
-        <v>28733741.706567012</v>
+        <v>20924527.338175468</v>
       </c>
       <c r="AR31" s="64">
         <f t="shared" si="18"/>
-        <v>70190793.295484543</v>
+        <v>35189373.707400247</v>
       </c>
       <c r="AX31" s="64">
         <f t="shared" si="19"/>
-        <v>452956861.64701688</v>
+        <v>3658520891.5827789</v>
       </c>
       <c r="AY31" s="48">
         <f t="shared" si="20"/>
-        <v>2968.244574684938</v>
+        <v>6558.9149264673797</v>
       </c>
       <c r="AZ31" s="14">
         <f t="shared" si="14"/>
-        <v>2464680250.0551219</v>
+        <v>5446191401.7889786</v>
       </c>
       <c r="BA31" s="65">
         <f t="shared" si="15"/>
@@ -3859,27 +3859,27 @@
       </c>
       <c r="AF32" s="64">
         <f t="shared" si="16"/>
-        <v>494219946.55014473</v>
+        <v>245195739.06693047</v>
       </c>
       <c r="AL32" s="64">
         <f t="shared" si="17"/>
-        <v>32984248.118405528</v>
+        <v>23278279.250937834</v>
       </c>
       <c r="AR32" s="64">
         <f t="shared" si="18"/>
-        <v>88725523.067535028</v>
+        <v>41045315.18779362</v>
       </c>
       <c r="AX32" s="64">
         <f t="shared" si="19"/>
-        <v>495861145.30289018</v>
+        <v>4477281615.6249981</v>
       </c>
       <c r="AY32" s="48">
         <f t="shared" si="20"/>
-        <v>3486.3940630192396</v>
+        <v>7571.8029261745905</v>
       </c>
       <c r="AZ32" s="14">
         <f t="shared" si="14"/>
-        <v>3136169175.4372315</v>
+        <v>6811179261.5289164</v>
       </c>
       <c r="BA32" s="65">
         <f t="shared" si="15"/>
@@ -3950,27 +3950,27 @@
       </c>
       <c r="AF33" s="64">
         <f t="shared" si="16"/>
-        <v>628525337.4805541</v>
+        <v>288239725.10989016</v>
       </c>
       <c r="AL33" s="64">
         <f t="shared" si="17"/>
-        <v>37685712.442599781</v>
+        <v>25753739.708090439</v>
       </c>
       <c r="AR33" s="64">
         <f t="shared" si="18"/>
-        <v>112274631.67894769</v>
+        <v>47725319.671577126</v>
       </c>
       <c r="AX33" s="64">
         <f t="shared" si="19"/>
-        <v>495861145.30289018</v>
+        <v>4477281615.6249981</v>
       </c>
       <c r="AY33" s="48">
         <f t="shared" si="20"/>
-        <v>4126.6887632796597</v>
+        <v>7806.3652518536455</v>
       </c>
       <c r="AZ33" s="14">
         <f t="shared" si="14"/>
-        <v>3997692702.3955197</v>
+        <v>7562346275.6050835</v>
       </c>
       <c r="BA33" s="65">
         <f t="shared" si="15"/>
@@ -4041,27 +4041,27 @@
       </c>
       <c r="AF34" s="64">
         <f t="shared" si="16"/>
-        <v>801792511.96554291</v>
+        <v>338389503.33337432</v>
       </c>
       <c r="AL34" s="64">
         <f t="shared" si="17"/>
-        <v>42891323.831077576</v>
+        <v>28358539.430361494</v>
       </c>
       <c r="AR34" s="64">
         <f t="shared" si="18"/>
-        <v>142389264.7799747</v>
+        <v>55372544.269987121</v>
       </c>
       <c r="AX34" s="64">
         <f t="shared" si="19"/>
-        <v>495861145.30289018</v>
+        <v>4477281615.6249981</v>
       </c>
       <c r="AY34" s="48">
         <f t="shared" si="20"/>
-        <v>5014.9266862804025</v>
+        <v>8306.5220084949069</v>
       </c>
       <c r="AZ34" s="14">
         <f t="shared" si="14"/>
-        <v>5205177019.6790686</v>
+        <v>8621644976.4583035</v>
       </c>
       <c r="BA34" s="65">
         <f t="shared" si="15"/>
@@ -4132,27 +4132,27 @@
       </c>
       <c r="AF35" s="64">
         <f t="shared" si="16"/>
-        <v>1027128237.6923612</v>
+        <v>397100360.91755426</v>
       </c>
       <c r="AL35" s="64">
         <f t="shared" si="17"/>
-        <v>48661188.894624561</v>
+        <v>31100873.174388409</v>
       </c>
       <c r="AR35" s="64">
         <f t="shared" si="18"/>
-        <v>181164310.16661745</v>
+        <v>64160018.906167388</v>
       </c>
       <c r="AX35" s="64">
         <f t="shared" si="19"/>
-        <v>495861145.30289018</v>
+        <v>4477281615.6249981</v>
       </c>
       <c r="AY35" s="48">
         <f t="shared" si="20"/>
-        <v>6270.668722122653</v>
+        <v>9176.2176930107053</v>
       </c>
       <c r="AZ35" s="14">
         <f t="shared" si="14"/>
-        <v>6942461766.0623312</v>
+        <v>10159289752.628944</v>
       </c>
       <c r="BA35" s="65">
         <f t="shared" si="15"/>
@@ -4223,27 +4223,27 @@
       </c>
       <c r="AF36" s="64">
         <f t="shared" si="16"/>
-        <v>1322699653.3105819</v>
+        <v>466187483.47488219</v>
       </c>
       <c r="AL36" s="64">
         <f t="shared" si="17"/>
-        <v>55063316.915649801</v>
+        <v>33989547.887325898</v>
       </c>
       <c r="AR36" s="64">
         <f t="shared" si="18"/>
-        <v>231452836.70505196</v>
+        <v>74297987.60863702</v>
       </c>
       <c r="AX36" s="64">
         <f t="shared" si="19"/>
-        <v>495861145.30289018</v>
+        <v>4477281615.6249981</v>
       </c>
       <c r="AY36" s="48">
         <f t="shared" si="20"/>
-        <v>8093.715799461449</v>
+        <v>10598.696308028551</v>
       </c>
       <c r="AZ36" s="14">
         <f t="shared" si="14"/>
-        <v>9520867655.2637615</v>
+        <v>12467547337.625431</v>
       </c>
       <c r="BA36" s="65">
         <f t="shared" si="15"/>
@@ -4353,7 +4353,7 @@
       </c>
       <c r="AF37" s="64">
         <f t="shared" si="16"/>
-        <v>1713958521.8476808</v>
+        <v>547931364.47813785</v>
       </c>
       <c r="AG37" s="11" t="s">
         <v>73</v>
@@ -4372,7 +4372,7 @@
       </c>
       <c r="AL37" s="64">
         <f t="shared" si="17"/>
-        <v>62174757.834079713</v>
+        <v>37034035.536313072</v>
       </c>
       <c r="AM37" s="11" t="s">
         <v>73</v>
@@ -4391,7 +4391,7 @@
       </c>
       <c r="AR37" s="64">
         <f t="shared" si="18"/>
-        <v>297175122.05525213</v>
+        <v>86043343.259294197</v>
       </c>
       <c r="AS37" s="11" t="s">
         <v>73</v>
@@ -4410,15 +4410,15 @@
       </c>
       <c r="AX37" s="64">
         <f t="shared" si="19"/>
-        <v>495861145.30289018</v>
+        <v>4477281615.6249981</v>
       </c>
       <c r="AY37" s="48">
         <f t="shared" si="20"/>
-        <v>10833.387930167843</v>
+        <v>12904.099092284661</v>
       </c>
       <c r="AZ37" s="14">
         <f t="shared" si="14"/>
-        <v>13493246564.177263</v>
+        <v>16072367376.036104</v>
       </c>
       <c r="BA37" s="65">
         <f t="shared" si="15"/>
@@ -4513,59 +4513,59 @@
       </c>
       <c r="Z38">
         <f>elasticity_mf*base_use_mf</f>
-        <v>-67499.324999999997</v>
+        <v>-112498.875</v>
       </c>
       <c r="AA38">
         <f>EXP((LN(base_use_mf/coeff_mf))/elasticity_mf)</f>
-        <v>650.00000000000114</v>
+        <v>650.00000000000057</v>
       </c>
       <c r="AB38">
         <f>elasticity_mf + 1</f>
-        <v>0.88</v>
+        <v>0.8</v>
       </c>
       <c r="AC38" s="11">
         <f>(Z38*AA38)/AB38</f>
-        <v>-49857455.965909176</v>
+        <v>-91405335.937500075</v>
       </c>
       <c r="AD38">
         <f>elasticity_mf*(base_use_mf-shortage_af_MF)</f>
-        <v>-38617.749409723176</v>
+        <v>-64362.915682871972</v>
       </c>
       <c r="AE38">
         <f>LN((base_use_mf-shortage_af_MF)/coeff_mf)</f>
-        <v>-1.3356422813261004</v>
+        <v>-1.853800070357275</v>
       </c>
       <c r="AF38" s="144">
         <f>IF(shortage_MF&lt;=lowerbound_MF,((elasticity_mf*base_use_mf*EXP((LN(base_use_mf/coeff_mf))/elasticity_mf))/(elasticity_mf + 1))-((elasticity_mf*(base_use_mf*(1-lowerbound_MF)*EXP((LN((base_use_mf*(1-lowerbound_MF)/coeff_mf))/elasticity_mf))/(elasticity_mf + 1)))), IF(shortage_MF&gt;=upperbound_MF,((elasticity_mf*base_use_mf*EXP((LN(base_use_mf/coeff_mf))/elasticity_mf))/(elasticity_mf + 1))-((elasticity_mf*(base_use_mf*(1-upperbound_MF))*EXP((LN((base_use_mf*(1-upperbound_MF))/coeff_mf))/elasticity_mf))/(elasticity_mf + 1)), ((elasticity_mf*base_use_mf*EXP((LN(base_use_mf/coeff_mf))/elasticity_mf))/(elasticity_mf + 1))-((elasticity_mf*(base_use_mf-shortage_af_MF)*EXP((AE38)/elasticity_mf))/(elasticity_mf + 1))))</f>
-        <v>2943474573.2709417</v>
+        <v>761736871.39212728</v>
       </c>
       <c r="AG38">
         <f>elasticity_ind*base_use_ind</f>
-        <v>-22499.775000000001</v>
+        <v>-44999.55</v>
       </c>
       <c r="AH38">
         <f>EXP((LN(base_use_ind/coeff_ind))/elasticity_ind)</f>
-        <v>649.99999999999932</v>
+        <v>650.00000000000057</v>
       </c>
       <c r="AI38">
         <f>elasticity_ind + 1</f>
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="AJ38" s="11">
         <f>(AG38*AH38)/AI38</f>
-        <v>-16249837.499999983</v>
+        <v>-36562134.37500003</v>
       </c>
       <c r="AK38">
         <f>elasticity_ind*(base_use_ind-shortage_af_IND)</f>
-        <v>-18488.445056905995</v>
+        <v>-36976.890113811991</v>
       </c>
       <c r="AL38" s="64">
         <f>IF(shortage_IND&lt;=lowerbound_IND,((elasticity_ind*base_use_ind*EXP((LN(base_use_ind/coeff_ind))/elasticity_ind))/(elasticity_ind + 1))-((elasticity_ind*(base_use_ind*(1-lowerbound_IND)*EXP((LN((base_use_ind*(1-lowerbound_IND)/coeff_ind))/elasticity_ind))/(elasticity_ind + 1)))), IF(shortage_IND&gt;=upperbound_IND,((elasticity_ind*base_use_ind*EXP((LN(base_use_ind/coeff_ind))/elasticity_ind))/(elasticity_ind + 1))-((elasticity_ind*(base_use_ind*(1-upperbound_IND))*EXP((LN((base_use_ind*(1-upperbound_IND))/coeff_ind))/elasticity_ind))/(elasticity_ind + 1)), ((elasticity_ind*base_use_ind*EXP((LN(base_use_ind/coeff_ind))/elasticity_ind))/(elasticity_ind + 1))-((elasticity_ind*(base_use_ind-shortage_af_IND)*EXP((LN((base_use_ind-shortage_af_IND)/coeff_ind))/elasticity_ind))/(elasticity_ind + 1))))</f>
-        <v>78887088.701905936</v>
+        <v>43632016.451510206</v>
       </c>
       <c r="AM38">
         <f>elasticity_comm*base_use_comm</f>
-        <v>-12374.876249999999</v>
+        <v>-22499.775000000001</v>
       </c>
       <c r="AN38">
         <f>EXP((LN(base_use_comm/coeff_comm))/elasticity_comm)</f>
@@ -4573,23 +4573,23 @@
       </c>
       <c r="AO38">
         <f>elasticity_comm + 1</f>
-        <v>0.89</v>
+        <v>0.8</v>
       </c>
       <c r="AP38" s="11">
         <f>(AM38*AN38)/AO38</f>
-        <v>-9037830.969101131</v>
+        <v>-18281067.187500015</v>
       </c>
       <c r="AQ38">
         <f>elasticity_comm*(base_use_comm-shortage_af_COM)</f>
-        <v>-7521.1670188562566</v>
+        <v>-13674.849125193194</v>
       </c>
       <c r="AR38" s="64">
         <f>IF(shortage_COM&lt;=lowerbound_COM,((elasticity_comm*base_use_comm*EXP((LN(base_use_comm/coeff_comm))/elasticity_comm))/(elasticity_comm + 1))-((elasticity_comm*(base_use_comm*(1-lowerbound_COM)*EXP((LN((base_use_comm*(1-lowerbound_COM)/coeff_comm))/elasticity_comm))/(elasticity_comm + 1)))), IF(shortage_COM&gt;=upperbound_COM,((elasticity_comm*base_use_comm*EXP((LN(base_use_comm/coeff_comm))/elasticity_comm))/(elasticity_comm + 1))-((elasticity_comm*(base_use_comm*(1-upperbound_COM))*EXP((LN((base_use_comm*(1-upperbound_COM))/coeff_comm))/elasticity_comm))/(elasticity_comm + 1)), ((elasticity_comm*base_use_comm*EXP((LN(base_use_comm/coeff_comm))/elasticity_comm))/(elasticity_comm + 1))-((elasticity_comm*(base_use_comm-shortage_af_COM)*EXP((LN((base_use_comm-shortage_af_COM)/coeff_comm))/elasticity_comm))/(elasticity_comm + 1))))</f>
-        <v>498851244.08505064</v>
+        <v>115694027.16101466</v>
       </c>
       <c r="AS38">
         <f>elasticity_lndscp*base_use_lndscp</f>
-        <v>-89999.1</v>
+        <v>-44999.55</v>
       </c>
       <c r="AT38">
         <f>EXP((LN(base_use_lndscp/coeff_lndscp))/elasticity_lndscp)</f>
@@ -4597,27 +4597,27 @@
       </c>
       <c r="AU38">
         <f>elasticity_lndscp + 1</f>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="AV38" s="11">
         <f>(AS38*AT38)/AU38</f>
-        <v>-97499025.000000089</v>
+        <v>-36562134.37500003</v>
       </c>
       <c r="AW38">
         <f>elasticity_lndscp*(base_use_lndscp-shortage_af_LNDSCP)</f>
-        <v>12690.946543206474</v>
+        <v>6345.4732716032368</v>
       </c>
       <c r="AX38" s="64">
         <f>IF(shortage_LNDSCP&lt;=$U$14,((elasticity_lndscp*base_use_lndscp*EXP((LN(base_use_lndscp/coeff_lndscp))/elasticity_lndscp))/(elasticity_lndscp + 1))-((elasticity_lndscp*(base_use_lndscp*(1-low_bound_lndscp)*EXP((LN((base_use_lndscp*(1-low_bound_lndscp)/coeff_lndscp))/elasticity_lndscp))/(elasticity_lndscp + 1)))), IF(shortage_LNDSCP&gt;=upperbound_LNDSCP,((elasticity_lndscp*base_use_lndscp*EXP((LN(base_use_lndscp/coeff_lndscp))/elasticity_lndscp))/(elasticity_lndscp + 1))-((elasticity_lndscp*(base_use_lndscp*(1-upperbound_LNDSCP))*EXP((LN((base_use_lndscp*(1-upperbound_LNDSCP))/coeff_lndscp))/elasticity_lndscp))/(elasticity_lndscp + 1)), ((elasticity_lndscp*base_use_lndscp*EXP((LN(base_use_lndscp/coeff_lndscp))/elasticity_lndscp))/(elasticity_lndscp + 1))-((elasticity_lndscp*(base_use_lndscp-shortage_af_LNDSCP)*EXP((LN((base_use_lndscp-shortage_af_LNDSCP)/coeff_lndscp))/elasticity_lndscp))/(elasticity_lndscp + 1))))</f>
-        <v>495861145.30289018</v>
+        <v>4477281615.6249981</v>
       </c>
       <c r="AY38" s="48">
         <f t="shared" si="20"/>
-        <v>19078.821907681722</v>
+        <v>20076.910468541635</v>
       </c>
       <c r="AZ38" s="144">
         <f t="shared" si="14"/>
-        <v>26403482129.485783</v>
+        <v>27784752608.754646</v>
       </c>
       <c r="BA38" s="65">
         <f t="shared" si="15"/>
@@ -4960,19 +4960,19 @@
       </c>
       <c r="R45" s="50">
         <f t="shared" ref="R45:R63" si="38">AF20/D45</f>
-        <v>712.02608956412109</v>
+        <v>686.31383242316451</v>
       </c>
       <c r="S45" s="50">
         <f t="shared" ref="S45:S63" si="39">AL20/F45</f>
-        <v>679.94725234587645</v>
+        <v>664.75116569798843</v>
       </c>
       <c r="T45" s="50">
         <f t="shared" ref="T45:T63" si="40">AR20/H45</f>
-        <v>711.98583096596383</v>
+        <v>683.16574641332227</v>
       </c>
       <c r="U45" s="50">
         <f t="shared" ref="U45:U63" si="41">AX20/J45</f>
-        <v>699.65362111474315</v>
+        <v>754.45046831970683</v>
       </c>
       <c r="V45" s="41"/>
       <c r="W45" s="41"/>
@@ -5047,19 +5047,19 @@
       </c>
       <c r="R46" s="50">
         <f t="shared" si="38"/>
-        <v>783.20054988361289</v>
+        <v>725.96229728625383</v>
       </c>
       <c r="S46" s="50">
         <f t="shared" si="39"/>
-        <v>711.9456498559814</v>
+        <v>680.04058835612602</v>
       </c>
       <c r="T46" s="50">
         <f t="shared" si="40"/>
-        <v>783.01147260005166</v>
+        <v>719.1056254713161</v>
       </c>
       <c r="U46" s="50">
         <f t="shared" si="41"/>
-        <v>756.86297016028038</v>
+        <v>888.03702820200306</v>
       </c>
       <c r="V46" s="41"/>
       <c r="W46" s="41"/>
@@ -5134,19 +5134,19 @@
       </c>
       <c r="R47" s="50">
         <f t="shared" si="38"/>
-        <v>865.2572307064346</v>
+        <v>769.3617258091283</v>
       </c>
       <c r="S47" s="50">
         <f t="shared" si="39"/>
-        <v>746.17347563082524</v>
+        <v>695.89787945164392</v>
       </c>
       <c r="T47" s="50">
         <f t="shared" si="40"/>
-        <v>864.75550662935916</v>
+        <v>758.13532682494645</v>
       </c>
       <c r="U47" s="50">
         <f t="shared" si="41"/>
-        <v>823.41368806109824</v>
+        <v>1062.2959450257169</v>
       </c>
       <c r="V47" s="41"/>
       <c r="W47" s="41"/>
@@ -5221,19 +5221,19 @@
       </c>
       <c r="R48" s="50">
         <f t="shared" si="38"/>
-        <v>960.32000025229956</v>
+        <v>816.98908705526526</v>
       </c>
       <c r="S48" s="50">
         <f t="shared" si="39"/>
-        <v>782.82318022574248</v>
+        <v>712.3509802167348</v>
       </c>
       <c r="T48" s="50">
         <f t="shared" si="40"/>
-        <v>959.263211697202</v>
+        <v>800.61111576639303</v>
       </c>
       <c r="U48" s="50">
         <f t="shared" si="41"/>
-        <v>901.67745784176077</v>
+        <v>1294.7902656972365</v>
       </c>
       <c r="V48" s="41"/>
       <c r="W48" s="41"/>
@@ -5308,19 +5308,19 @@
       </c>
       <c r="R49" s="50">
         <f t="shared" si="38"/>
-        <v>1071.0100156205006</v>
+        <v>869.39711009765369</v>
       </c>
       <c r="S49" s="50">
         <f t="shared" si="39"/>
-        <v>822.10659599861606</v>
+        <v>729.42952366326165</v>
       </c>
       <c r="T49" s="50">
         <f t="shared" si="40"/>
-        <v>1069.044204483489</v>
+        <v>846.940452179776</v>
       </c>
       <c r="U49" s="50">
         <f t="shared" si="41"/>
-        <v>994.8746116710181</v>
+        <v>1613.1373849124095</v>
       </c>
       <c r="V49" s="41"/>
       <c r="W49" s="41"/>
@@ -5395,19 +5395,19 @@
       </c>
       <c r="R50" s="50">
         <f t="shared" si="38"/>
-        <v>1200.5811621065909</v>
+        <v>927.22874226141789</v>
       </c>
       <c r="S50" s="50">
         <f t="shared" si="39"/>
-        <v>864.25714807086797</v>
+        <v>747.16495576574005</v>
       </c>
       <c r="T50" s="50">
         <f t="shared" si="40"/>
-        <v>1197.194148954329</v>
+        <v>897.59080835945201</v>
       </c>
       <c r="U50" s="50">
         <f t="shared" si="41"/>
-        <v>1107.4809275953969</v>
+        <v>2062.3996698995493</v>
       </c>
       <c r="V50" s="41"/>
       <c r="W50" s="41"/>
@@ -5482,19 +5482,19 @@
       </c>
       <c r="R51" s="50">
         <f t="shared" si="38"/>
-        <v>1353.0976106635433</v>
+        <v>991.23484258243843</v>
       </c>
       <c r="S51" s="50">
         <f t="shared" si="39"/>
-        <v>909.53234596395259</v>
+        <v>765.59066666018964</v>
       </c>
       <c r="T51" s="50">
         <f t="shared" si="40"/>
-        <v>1347.5526419659211</v>
+        <v>953.10026314547542</v>
       </c>
       <c r="U51" s="50">
         <f t="shared" si="41"/>
-        <v>1245.8882214519051</v>
+        <v>2719.3391982580661</v>
       </c>
       <c r="V51" s="41"/>
       <c r="W51" s="41"/>
@@ -5569,19 +5569,19 @@
       </c>
       <c r="R52" s="50">
         <f t="shared" si="38"/>
-        <v>1533.6682628385406</v>
+        <v>1062.2959450257174</v>
       </c>
       <c r="S52" s="50">
         <f t="shared" si="39"/>
-        <v>958.21659509421215</v>
+        <v>784.74213279750245</v>
       </c>
       <c r="T52" s="50">
         <f t="shared" si="40"/>
-        <v>1524.9093232886014</v>
+        <v>1014.0902838039974</v>
       </c>
       <c r="U52" s="50">
         <f t="shared" si="41"/>
-        <v>1419.5215186730529</v>
+        <v>3721.5376659196286</v>
       </c>
       <c r="V52" s="41"/>
       <c r="W52" s="41"/>
@@ -5656,19 +5656,19 @@
       </c>
       <c r="R53" s="50">
         <f t="shared" si="38"/>
-        <v>1748.7586402698719</v>
+        <v>1141.4491711053656</v>
       </c>
       <c r="S53" s="50">
         <f t="shared" si="39"/>
-        <v>1010.624373271579</v>
+        <v>804.65707108832135</v>
       </c>
       <c r="T53" s="50">
         <f t="shared" si="40"/>
-        <v>1735.2747150774885</v>
+        <v>1081.2812152754052</v>
       </c>
       <c r="U53" s="50">
         <f t="shared" si="41"/>
-        <v>1642.8215766435719</v>
+        <v>5331.0913514836884</v>
       </c>
       <c r="V53" s="42"/>
       <c r="W53" s="42"/>
@@ -5743,19 +5743,19 @@
       </c>
       <c r="R54" s="50">
         <f t="shared" si="38"/>
-        <v>2006.6090810514656</v>
+        <v>1229.9216978214797</v>
       </c>
       <c r="S54" s="50">
         <f t="shared" si="39"/>
-        <v>1067.1038242936959</v>
+        <v>825.37560618636269</v>
       </c>
       <c r="T54" s="50">
         <f t="shared" si="40"/>
-        <v>1986.2385722343481</v>
+        <v>1155.5111366008798</v>
       </c>
       <c r="U54" s="50">
         <f t="shared" si="41"/>
-        <v>1938.9734896890113</v>
+        <v>8085.9604325751707</v>
       </c>
       <c r="V54" s="41"/>
       <c r="W54" s="41"/>
@@ -5830,19 +5830,19 @@
       </c>
       <c r="R55" s="50">
         <f t="shared" si="38"/>
-        <v>2317.8001369653712</v>
+        <v>1329.1726243698765</v>
       </c>
       <c r="S55" s="50">
         <f t="shared" si="39"/>
-        <v>1128.0408288299159</v>
+        <v>846.94045217977634</v>
       </c>
       <c r="T55" s="50">
         <f t="shared" si="40"/>
-        <v>2287.4474364334533</v>
+        <v>1237.7589270744008</v>
       </c>
       <c r="U55" s="50">
         <f t="shared" si="41"/>
-        <v>2347.4396939333778</v>
+        <v>13198.463623396112</v>
       </c>
       <c r="V55" s="41"/>
       <c r="W55" s="41"/>
@@ -5917,19 +5917,19 @@
       </c>
       <c r="R56" s="50">
         <f t="shared" si="38"/>
-        <v>2696.0236711098801</v>
+        <v>1440.945672389603</v>
       </c>
       <c r="S56" s="50">
         <f t="shared" si="39"/>
-        <v>1193.8636222575726</v>
+        <v>869.39711009765313</v>
       </c>
       <c r="T56" s="50">
         <f t="shared" si="40"/>
-        <v>2651.2458478777321</v>
+        <v>1329.1726243698768</v>
       </c>
       <c r="U56" s="50">
         <f t="shared" si="41"/>
-        <v>2940.6233722030502</v>
+        <v>23751.339150405194</v>
       </c>
       <c r="V56" s="41"/>
       <c r="W56" s="41"/>
@@ -6004,19 +6004,19 @@
       </c>
       <c r="R57" s="50">
         <f t="shared" si="38"/>
-        <v>3159.1441898934386</v>
+        <v>1567.3359601671345</v>
       </c>
       <c r="S57" s="50">
         <f t="shared" si="39"/>
-        <v>1265.048040193074</v>
+        <v>892.79408279231507</v>
       </c>
       <c r="T57" s="50">
         <f t="shared" si="40"/>
-        <v>3093.5441081608674</v>
+        <v>1431.1044734011321</v>
       </c>
       <c r="U57" s="50">
         <f t="shared" si="41"/>
-        <v>2971.5328426499054</v>
+        <v>26830.876935307166</v>
       </c>
       <c r="V57" s="41"/>
       <c r="W57" s="41"/>
@@ -6091,19 +6091,19 @@
       </c>
       <c r="R58" s="50">
         <f t="shared" si="38"/>
-        <v>3730.6738723917438</v>
+        <v>1710.8751983862787</v>
       </c>
       <c r="S58" s="50">
         <f t="shared" si="39"/>
-        <v>1342.1234854490674</v>
+        <v>917.18310893065632</v>
       </c>
       <c r="T58" s="50">
         <f t="shared" si="40"/>
-        <v>3635.0023832211177</v>
+        <v>1545.1544854963138</v>
       </c>
       <c r="U58" s="50">
         <f t="shared" si="41"/>
-        <v>2759.2804967463403</v>
+        <v>24914.385725642365</v>
       </c>
       <c r="V58" s="41"/>
       <c r="W58" s="41"/>
@@ -6178,19 +6178,19 @@
       </c>
       <c r="R59" s="50">
         <f t="shared" si="38"/>
-        <v>4441.8436573491754</v>
+        <v>1874.6411904124654</v>
       </c>
       <c r="S59" s="50">
         <f t="shared" si="39"/>
-        <v>1425.6797253993479</v>
+        <v>942.61941802108777</v>
       </c>
       <c r="T59" s="50">
         <f t="shared" si="40"/>
-        <v>4302.66055482301</v>
+        <v>1673.2248910675694</v>
       </c>
       <c r="U59" s="50">
         <f t="shared" si="41"/>
-        <v>2575.3284636299177</v>
+        <v>23253.426677266209</v>
       </c>
       <c r="V59" s="41"/>
       <c r="W59" s="41"/>
@@ -6265,19 +6265,19 @@
       </c>
       <c r="R60" s="50">
         <f t="shared" si="38"/>
-        <v>5334.5429691035642</v>
+        <v>2062.3996698995447</v>
       </c>
       <c r="S60" s="50">
         <f t="shared" si="39"/>
-        <v>1516.3746466706866</v>
+        <v>969.16200862023595</v>
       </c>
       <c r="T60" s="50">
         <f t="shared" si="40"/>
-        <v>5132.2022009093434</v>
+        <v>1817.5886295583018</v>
       </c>
       <c r="U60" s="50">
         <f t="shared" si="41"/>
-        <v>2414.3704346530476</v>
+        <v>21800.087509937068</v>
       </c>
       <c r="V60" s="41"/>
       <c r="W60" s="41"/>
@@ -6352,19 +6352,19 @@
       </c>
       <c r="R61" s="50">
         <f t="shared" si="38"/>
-        <v>6465.5406970925205</v>
+        <v>2278.789549341665</v>
       </c>
       <c r="S61" s="50">
         <f t="shared" si="39"/>
-        <v>1614.9431152142658</v>
+        <v>996.87395210806267</v>
       </c>
       <c r="T61" s="50">
         <f t="shared" si="40"/>
-        <v>6171.1298270452899</v>
+        <v>1980.9760552011996</v>
       </c>
       <c r="U61" s="50">
         <f t="shared" si="41"/>
-        <v>2272.3486443793386</v>
+        <v>20517.729421117238</v>
       </c>
       <c r="V61" s="41"/>
       <c r="W61" s="41"/>
@@ -6439,19 +6439,19 @@
       </c>
       <c r="R62" s="50">
         <f t="shared" si="38"/>
-        <v>7912.6204469091936</v>
+        <v>2529.5670010723097</v>
       </c>
       <c r="S62" s="50">
         <f t="shared" si="39"/>
-        <v>1722.207114752877</v>
+        <v>1025.8227246956724</v>
       </c>
       <c r="T62" s="50">
         <f t="shared" si="40"/>
-        <v>7483.2635587477707</v>
+        <v>2166.6854568175727</v>
       </c>
       <c r="U62" s="50">
         <f t="shared" si="41"/>
-        <v>2146.1070530249308</v>
+        <v>19377.855564388501</v>
       </c>
       <c r="V62" s="41"/>
       <c r="W62" s="41"/>
@@ -6526,19 +6526,19 @@
       </c>
       <c r="R63" s="50">
         <f t="shared" si="38"/>
-        <v>12229.897699905789</v>
+        <v>3164.9548108783647</v>
       </c>
       <c r="S63" s="50">
         <f t="shared" si="39"/>
-        <v>1966.6166647308698</v>
+        <v>1087.7248999972071</v>
       </c>
       <c r="T63" s="50">
         <f t="shared" si="40"/>
-        <v>11305.562118565322</v>
+        <v>2621.9960886633216</v>
       </c>
       <c r="U63" s="50">
         <f t="shared" si="41"/>
-        <v>1931.496347722438</v>
+        <v>17440.070007949656</v>
       </c>
       <c r="V63" s="41"/>
       <c r="W63" s="41"/>
@@ -6635,12 +6635,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Metadata xmlns="c8a5693f-cb4f-4469-ad8f-971ccdc8dc5c" xsi:nil="true"/>
-    <Notes xmlns="c8a5693f-cb4f-4469-ad8f-971ccdc8dc5c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6874,28 +6874,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Metadata xmlns="c8a5693f-cb4f-4469-ad8f-971ccdc8dc5c" xsi:nil="true"/>
+    <Notes xmlns="c8a5693f-cb4f-4469-ad8f-971ccdc8dc5c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB85D8AC-4DEA-4D66-8105-40ECD4B542B0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BEF16BB-3AEF-4926-94B8-DF9556B55AE8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8ca2015b-1270-41a8-9966-06a19c2d4f3a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="C8A5693F-CB4F-4469-AD8F-971CCDC8DC5C"/>
-    <ds:schemaRef ds:uri="c8a5693f-cb4f-4469-ad8f-971ccdc8dc5c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6921,9 +6911,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BEF16BB-3AEF-4926-94B8-DF9556B55AE8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB85D8AC-4DEA-4D66-8105-40ECD4B542B0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8ca2015b-1270-41a8-9966-06a19c2d4f3a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="C8A5693F-CB4F-4469-AD8F-971CCDC8DC5C"/>
+    <ds:schemaRef ds:uri="c8a5693f-cb4f-4469-ad8f-971ccdc8dc5c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>